<commit_message>
Apresentação e Elaborar Drigrama de Classes
</commit_message>
<xml_diff>
--- a/documentos/TEMPLATE_Transacoes.xlsx
+++ b/documentos/TEMPLATE_Transacoes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\GitHub\LPA\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70103D2C-8514-4372-8BFE-7BF979871D9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D4C531-30C3-47F1-97D8-CBFB0BB93D46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Manutenção de Cadastros</t>
   </si>
@@ -275,7 +275,28 @@
     <t>Entrega</t>
   </si>
   <si>
-    <t>xxxx</t>
+    <t>Listagem de Clientes</t>
+  </si>
+  <si>
+    <t>Listagem de Bairros</t>
+  </si>
+  <si>
+    <t>Listagem de Produtos</t>
+  </si>
+  <si>
+    <t>Listagem de Entregas</t>
+  </si>
+  <si>
+    <t>Listagem de entregas: Quantidade Totalização</t>
+  </si>
+  <si>
+    <t>Listagem de Pedidos</t>
+  </si>
+  <si>
+    <t>Listagem com totalização e filtro</t>
+  </si>
+  <si>
+    <t>Listagem com totalização por mês</t>
   </si>
 </sst>
 </file>
@@ -326,7 +347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -349,11 +370,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -380,6 +412,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,15 +757,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
@@ -986,13 +1024,13 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="8">
-        <f>SUM(B16:F20)</f>
-        <v>5</v>
+        <f>SUM(B16:F23)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
@@ -1005,7 +1043,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
@@ -1018,7 +1056,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
@@ -1030,30 +1068,69 @@
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>21</v>
+      <c r="A20" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="8"/>
     </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="8"/>
+    </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B25" s="2">
         <f>G3+G10+G16</f>
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="G16:G20"/>
+    <mergeCell ref="G16:G23"/>
     <mergeCell ref="A14:F14"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A8:F8"/>

</xml_diff>